<commit_message>
testing key number bug
key can only accept 3
</commit_message>
<xml_diff>
--- a/python_backend/words.xlsx
+++ b/python_backend/words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamlinliu/Documents/GitHub/Caesar_cipher/python_backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42967E22-0CA7-3247-BC3B-D11BE2845119}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A92EF5B-DCC6-C046-8B3C-E2858C5B2293}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{990AE4D7-93C8-5C44-AA8C-E84F1F01553E}"/>
   </bookViews>
@@ -3028,6 +3028,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="\'@\'\,"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3063,9 +3066,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3383,12 +3387,12 @@
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="21.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17" x14ac:dyDescent="0.2">

</xml_diff>